<commit_message>
Se añade nueva pagina que presenta las transacciones del dia de Acciones, Bonos, Obligaciones, Papeles Comerciales y última fecha de venta de acciones
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="121">
   <si>
     <t>variation</t>
   </si>
@@ -336,6 +336,57 @@
   </si>
   <si>
     <t>API</t>
+  </si>
+  <si>
+    <t>shareslastdate</t>
+  </si>
+  <si>
+    <t>ShareslastdateController</t>
+  </si>
+  <si>
+    <t>SP_SHARESLASTDATE_SELECT</t>
+  </si>
+  <si>
+    <t>SP_BONDHIS_SELECT</t>
+  </si>
+  <si>
+    <t>historicobonos</t>
+  </si>
+  <si>
+    <t>BondshisController</t>
+  </si>
+  <si>
+    <t>ShareshisController</t>
+  </si>
+  <si>
+    <t>historicoacciones</t>
+  </si>
+  <si>
+    <t>SP_SHARES_SELECT</t>
+  </si>
+  <si>
+    <t>dailyoverview-page</t>
+  </si>
+  <si>
+    <t>ConsultarAccionesDelDia</t>
+  </si>
+  <si>
+    <t>ConsultarBonosDelDia</t>
+  </si>
+  <si>
+    <t>ConsultarUltimaFechaAcciones</t>
+  </si>
+  <si>
+    <t>SP_OBLIGACIONESHIS_SELECT</t>
+  </si>
+  <si>
+    <t>historicoobligaciones</t>
+  </si>
+  <si>
+    <t>ObligacioneshisController</t>
+  </si>
+  <si>
+    <t>ConsultarObligacionesDelDia</t>
   </si>
 </sst>
 </file>
@@ -379,7 +430,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -561,11 +612,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -588,6 +670,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,6 +1508,74 @@
       <c r="H22" s="8"/>
       <c r="I22" s="11"/>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C27">
     <sortCondition ref="B2:B27"/>

</xml_diff>

<commit_message>
Se añaden tablas de valores genericos y facturas comerciales del día
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
   <si>
     <t>variation</t>
   </si>
@@ -387,6 +387,30 @@
   </si>
   <si>
     <t>ConsultarObligacionesDelDia</t>
+  </si>
+  <si>
+    <t>SP_FACTURASHIS_SELECT</t>
+  </si>
+  <si>
+    <t>historicofacturas</t>
+  </si>
+  <si>
+    <t>FacturashisController</t>
+  </si>
+  <si>
+    <t>ConsultarFacturasDelDia</t>
+  </si>
+  <si>
+    <t>historicogenericos</t>
+  </si>
+  <si>
+    <t>GenericoshisController</t>
+  </si>
+  <si>
+    <t>SP_GENERICOSSHIS_SELECT</t>
+  </si>
+  <si>
+    <t>ConsultarGenericosDelDia</t>
   </si>
 </sst>
 </file>
@@ -988,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,6 +1600,40 @@
         <v>120</v>
       </c>
     </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C27">
     <sortCondition ref="B2:B27"/>

</xml_diff>

<commit_message>
Se añaden gráficos relacionados con Rendimientos y Tasas de bonos
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
   <si>
     <t>variation</t>
   </si>
@@ -411,6 +411,15 @@
   </si>
   <si>
     <t>ConsultarGenericosDelDia</t>
+  </si>
+  <si>
+    <t>SP_BONOSHIS_RESUMEN_SELECT</t>
+  </si>
+  <si>
+    <t>BonoshisresumenController</t>
+  </si>
+  <si>
+    <t>bonoshisresumen</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,6 +1643,17 @@
         <v>128</v>
       </c>
     </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C27">
     <sortCondition ref="B2:B27"/>

</xml_diff>

<commit_message>
Nueva tabla de dividendos en la pantalla de acciones
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="137">
   <si>
     <t>variation</t>
   </si>
@@ -420,6 +420,21 @@
   </si>
   <si>
     <t>bonoshisresumen</t>
+  </si>
+  <si>
+    <t>SP_DIVIDENDOS_SELECT</t>
+  </si>
+  <si>
+    <t>dividendos</t>
+  </si>
+  <si>
+    <t>DividendosController</t>
+  </si>
+  <si>
+    <t>ObtenerDividendos</t>
+  </si>
+  <si>
+    <t>emisor</t>
   </si>
 </sst>
 </file>
@@ -680,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -707,6 +722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,6 +1670,26 @@
         <v>129</v>
       </c>
     </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C27">
     <sortCondition ref="B2:B27"/>

</xml_diff>

<commit_message>
Primera version del simulador de acciones
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="141">
   <si>
     <t>variation</t>
   </si>
@@ -435,6 +435,18 @@
   </si>
   <si>
     <t>emisor</t>
+  </si>
+  <si>
+    <t>simulacion</t>
+  </si>
+  <si>
+    <t>SimulacionController</t>
+  </si>
+  <si>
+    <t>SP_DIVIDENDOSHIS_SELECT</t>
+  </si>
+  <si>
+    <t>$emisor,$precio,$capita</t>
   </si>
 </sst>
 </file>
@@ -1037,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,6 +1702,23 @@
         <v>135</v>
       </c>
     </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C27">
     <sortCondition ref="B2:B27"/>

</xml_diff>

<commit_message>
Cambio de estilos en tablas CRUD
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -490,7 +490,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -520,126 +520,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -652,9 +536,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -667,39 +549,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -707,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -715,26 +564,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1052,7 +885,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,62 +900,62 @@
     <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="7" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="16"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1142,10 +975,10 @@
         <v>71</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="6"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1165,10 +998,10 @@
         <v>71</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1188,10 +1021,10 @@
         <v>72</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="6"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1209,10 +1042,10 @@
       <c r="H6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1232,10 +1065,10 @@
       <c r="H7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1251,10 +1084,10 @@
         <v>75</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="6"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1274,10 +1107,10 @@
       <c r="H9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1297,10 +1130,10 @@
       <c r="H10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1318,10 +1151,10 @@
       <c r="H11" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1341,10 +1174,10 @@
       <c r="H12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1362,12 +1195,12 @@
       <c r="H13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1385,10 +1218,10 @@
       <c r="H14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1410,10 +1243,10 @@
       <c r="H15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1435,10 +1268,10 @@
       <c r="H16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1456,10 +1289,10 @@
       <c r="H17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I17" s="6"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1475,10 +1308,10 @@
         <v>88</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="6"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1500,10 +1333,10 @@
       <c r="H19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I19" s="6"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1521,12 +1354,12 @@
       <c r="H20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1548,176 +1381,213 @@
       <c r="H21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="9" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="11"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H23" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="2" t="s">
         <v>115</v>
       </c>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="23" t="s">
+      <c r="H26" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="23" t="s">
+      <c r="H27" s="2" t="s">
         <v>124</v>
       </c>
+      <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H28" s="23" t="s">
+      <c r="H28" s="2" t="s">
         <v>128</v>
       </c>
+      <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="2" t="s">
         <v>129</v>
       </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G30" s="24" t="s">
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H30" s="24" t="s">
+      <c r="H30" s="2" t="s">
         <v>135</v>
       </c>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G31" s="24" t="s">
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:C27">

</xml_diff>

<commit_message>
Pequeños cambios en formato y se cambia localhost por 127.0.0.1
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -470,7 +470,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -486,6 +486,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -568,6 +574,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,7 +892,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1058,7 @@
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="9" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1093,7 +1100,7 @@
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="9" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1116,7 +1123,7 @@
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1183,7 +1190,7 @@
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="9" t="s">
         <v>65</v>
       </c>
       <c r="D13" s="2"/>
@@ -1206,7 +1213,7 @@
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D14" s="2"/>
@@ -1342,7 +1349,7 @@
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="9" t="s">
         <v>70</v>
       </c>
       <c r="D20" s="2"/>

</xml_diff>

<commit_message>
Nuevos graficos de interes y recupearcion anual
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="142">
   <si>
     <t>variation</t>
   </si>
@@ -447,6 +447,9 @@
   </si>
   <si>
     <t>$emisor,$precio,$capita</t>
+  </si>
+  <si>
+    <t>SP_RECUPERACION_ANUAL</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -558,11 +561,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -575,6 +589,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,6 +1611,11 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C27">
     <sortCondition ref="B2:B27"/>

</xml_diff>

<commit_message>
cambios a shares y variation
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\SFEInvestment\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9B23DF-C798-44A6-ABDF-0687EDDC8916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="10665"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="148">
   <si>
     <t>variation</t>
   </si>
@@ -450,12 +451,30 @@
   </si>
   <si>
     <t>SP_RECUPERACION_ANUAL</t>
+  </si>
+  <si>
+    <t>SP_ACTUALIZAR_AMORTIZACION_INVESTMENT</t>
+  </si>
+  <si>
+    <t>SP_ACTUALIZAR_CONSOLIDADO_INVERSIONES</t>
+  </si>
+  <si>
+    <t>SP_AMORTIZATION_BY_OWNER</t>
+  </si>
+  <si>
+    <t>SP_BOND_AMORTIZATION_CREATION</t>
+  </si>
+  <si>
+    <t>SP_INVESTMENT_BY_OWNER</t>
+  </si>
+  <si>
+    <t>recuperacionanual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -473,7 +492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,7 +513,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -587,9 +612,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,18 +929,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
@@ -958,7 +984,7 @@
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -983,7 +1009,7 @@
       <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1006,7 +1032,7 @@
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1073,7 +1099,7 @@
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1115,7 +1141,7 @@
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1138,7 +1164,7 @@
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1205,7 +1231,7 @@
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D13" s="2"/>
@@ -1228,7 +1254,7 @@
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D14" s="2"/>
@@ -1249,7 +1275,7 @@
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1274,7 +1300,7 @@
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="10" t="s">
         <v>67</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1364,7 +1390,7 @@
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D20" s="2"/>
@@ -1425,10 +1451,10 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1446,10 +1472,10 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1467,10 +1493,10 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1488,10 +1514,10 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1509,10 +1535,10 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1530,10 +1556,10 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1551,10 +1577,10 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1568,10 +1594,10 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1591,10 +1617,10 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1612,12 +1638,90 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="10" t="s">
+      <c r="A32" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>141</v>
       </c>
     </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:C27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C27">
     <sortCondition ref="B2:B27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nueva adicion de columnas para diferencia premio
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\SFEInvestment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9B23DF-C798-44A6-ABDF-0687EDDC8916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFB9D5D-38AE-4AA5-8847-3CE5EE0D7E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24330" yWindow="1830" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -615,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,7 +933,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se añade funcionalidad para mantenimiento de inversiones
</commit_message>
<xml_diff>
--- a/RelacionFrontBack.xlsx
+++ b/RelacionFrontBack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\SFEInvestment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFB9D5D-38AE-4AA5-8847-3CE5EE0D7E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76402811-B990-47AE-AE38-9573E6864C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24330" yWindow="1830" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="149">
   <si>
     <t>variation</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>recuperacionanual</t>
+  </si>
+  <si>
+    <t>Bonos - Inversiones - Acciones</t>
   </si>
 </sst>
 </file>
@@ -933,7 +936,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1269,9 @@
       <c r="H14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">

</xml_diff>